<commit_message>
File Path input to Added from arguments
</commit_message>
<xml_diff>
--- a/Docs/6E25.xlsx
+++ b/Docs/6E25.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Sheet4!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -4022,6 +4022,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4069,7 +4072,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4104,7 +4107,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>

</xml_diff>